<commit_message>
Finalización de 100 horas
</commit_message>
<xml_diff>
--- a/Recursos/HORAS PRÁCTICAS Carlos Valladarez.xlsx
+++ b/Recursos/HORAS PRÁCTICAS Carlos Valladarez.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\carlos\Documents\Vinculación y practicas\Vin-Prac\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\carlo\Documents\GitHub\Vin-Prac\Recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A3AF8D-854C-41F7-87B7-7A3EC02DD79E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05635B13-9E13-4502-A29C-B56A0D5A93D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Carlos Valladarez" sheetId="1" r:id="rId1"/>
@@ -1190,20 +1190,20 @@
   </sheetPr>
   <dimension ref="B1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="67.85546875" customWidth="1"/>
+    <col min="1" max="1" width="1.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="67.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="46"/>
       <c r="C1" s="40" t="s">
         <v>0</v>
@@ -1212,7 +1212,7 @@
       <c r="E1" s="41"/>
       <c r="F1" s="42"/>
     </row>
-    <row r="2" spans="2:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="47"/>
       <c r="C2" s="43" t="s">
         <v>24</v>
@@ -1221,7 +1221,7 @@
       <c r="E2" s="44"/>
       <c r="F2" s="45"/>
     </row>
-    <row r="3" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="47"/>
       <c r="C3" s="48" t="s">
         <v>28</v>
@@ -1230,14 +1230,14 @@
       <c r="E3" s="49"/>
       <c r="F3" s="50"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="11"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="13"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="14" t="s">
         <v>1</v>
       </c>
@@ -1248,7 +1248,7 @@
       <c r="E5" s="55"/>
       <c r="F5" s="56"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="14" t="s">
         <v>2</v>
       </c>
@@ -1259,7 +1259,7 @@
       <c r="E6" s="15"/>
       <c r="F6" s="16"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="14" t="s">
         <v>24</v>
       </c>
@@ -1268,12 +1268,12 @@
       <c r="E7" s="12"/>
       <c r="F7" s="13"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="12">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>3</v>
@@ -1283,21 +1283,21 @@
       </c>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="14"/>
       <c r="C9" s="12"/>
       <c r="D9" s="17"/>
       <c r="E9" s="18"/>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="19"/>
       <c r="C10" s="20"/>
       <c r="D10" s="21"/>
       <c r="E10" s="22"/>
       <c r="F10" s="23"/>
     </row>
-    <row r="11" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B11" s="38" t="s">
         <v>5</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="39"/>
       <c r="C12" s="9" t="s">
         <v>8</v>
@@ -1323,7 +1323,7 @@
       </c>
       <c r="F12" s="52"/>
     </row>
-    <row r="13" spans="2:6" s="26" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" s="26" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="30">
         <v>44984</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="30">
         <v>44985</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="2:6" s="26" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" s="26" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="30">
         <v>44986</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="30">
         <v>44987</v>
       </c>
@@ -1391,7 +1391,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:6" s="26" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" s="26" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B17" s="30">
         <v>44988</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="30">
         <v>44991</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="2:6" s="26" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" s="26" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="30">
         <v>44992</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="30">
         <v>44993</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="2:6" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B21" s="30">
         <v>44994</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="30">
         <v>44995</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="2:6" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B23" s="30">
         <v>44998</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" s="30">
         <v>44999</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="2:6" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B25" s="30">
         <v>45000</v>
       </c>
@@ -1544,153 +1544,153 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" s="27"/>
       <c r="C26" s="28"/>
       <c r="D26" s="28"/>
       <c r="E26" s="26"/>
       <c r="F26" s="29"/>
     </row>
-    <row r="27" spans="2:6" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B27" s="27"/>
       <c r="C27" s="28"/>
       <c r="D27" s="28"/>
       <c r="F27" s="25"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" s="27"/>
       <c r="C28" s="28"/>
       <c r="D28" s="28"/>
       <c r="E28" s="26"/>
       <c r="F28" s="29"/>
     </row>
-    <row r="29" spans="2:6" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B29" s="27"/>
       <c r="C29" s="28"/>
       <c r="D29" s="28"/>
       <c r="F29" s="25"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" s="27"/>
       <c r="C30" s="28"/>
       <c r="D30" s="28"/>
       <c r="E30" s="26"/>
       <c r="F30" s="29"/>
     </row>
-    <row r="31" spans="2:6" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B31" s="27"/>
       <c r="C31" s="28"/>
       <c r="D31" s="28"/>
       <c r="F31" s="25"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B32" s="27"/>
       <c r="C32" s="28"/>
       <c r="D32" s="28"/>
       <c r="E32" s="26"/>
       <c r="F32" s="29"/>
     </row>
-    <row r="33" spans="2:6" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:6" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B33" s="27"/>
       <c r="C33" s="28"/>
       <c r="D33" s="28"/>
       <c r="F33" s="25"/>
     </row>
-    <row r="34" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="27"/>
       <c r="C34" s="28"/>
       <c r="D34" s="28"/>
       <c r="E34" s="26"/>
       <c r="F34" s="29"/>
     </row>
-    <row r="35" spans="2:6" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B35" s="27"/>
       <c r="C35" s="28"/>
       <c r="D35" s="28"/>
       <c r="F35" s="25"/>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36" s="27"/>
       <c r="C36" s="28"/>
       <c r="D36" s="28"/>
       <c r="E36" s="26"/>
       <c r="F36" s="29"/>
     </row>
-    <row r="37" spans="2:6" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:6" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B37" s="27"/>
       <c r="C37" s="28"/>
       <c r="D37" s="28"/>
       <c r="F37" s="25"/>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B38" s="27"/>
       <c r="C38" s="28"/>
       <c r="D38" s="28"/>
       <c r="E38" s="26"/>
       <c r="F38" s="29"/>
     </row>
-    <row r="39" spans="2:6" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:6" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B39" s="27"/>
       <c r="C39" s="28"/>
       <c r="D39" s="28"/>
       <c r="F39" s="25"/>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" s="27"/>
       <c r="C40" s="28"/>
       <c r="D40" s="28"/>
       <c r="E40" s="26"/>
       <c r="F40" s="29"/>
     </row>
-    <row r="41" spans="2:6" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:6" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B41" s="27"/>
       <c r="C41" s="28"/>
       <c r="D41" s="28"/>
       <c r="F41" s="25"/>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B42" s="27"/>
       <c r="C42" s="28"/>
       <c r="D42" s="28"/>
       <c r="E42" s="26"/>
       <c r="F42" s="29"/>
     </row>
-    <row r="43" spans="2:6" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:6" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B43" s="27"/>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
       <c r="F43" s="25"/>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B44" s="27"/>
       <c r="C44" s="28"/>
       <c r="D44" s="28"/>
       <c r="E44" s="26"/>
       <c r="F44" s="29"/>
     </row>
-    <row r="45" spans="2:6" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:6" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B45" s="27"/>
       <c r="C45" s="28"/>
       <c r="D45" s="28"/>
       <c r="F45" s="25"/>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B46" s="27"/>
       <c r="C46" s="28"/>
       <c r="D46" s="28"/>
       <c r="E46" s="26"/>
       <c r="F46" s="29"/>
     </row>
-    <row r="47" spans="2:6" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:6" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B47" s="27"/>
       <c r="C47" s="28"/>
       <c r="D47" s="28"/>
       <c r="F47" s="25"/>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F48" s="29"/>
     </row>
-    <row r="49" spans="2:6" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:6" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B49" s="36" t="s">
         <v>22</v>
       </c>
@@ -1702,7 +1702,7 @@
       </c>
       <c r="F49" s="23"/>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="10"/>
@@ -1735,15 +1735,15 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="7.7109375" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="72.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="72.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.3">
       <c r="A1" s="57" t="s">
         <v>10</v>
       </c>
@@ -1752,7 +1752,7 @@
       <c r="D1" s="57"/>
       <c r="E1" s="57"/>
     </row>
-    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="58" t="s">
         <v>11</v>
       </c>
@@ -1761,12 +1761,12 @@
       <c r="D2" s="58"/>
       <c r="E2" s="58"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1774,19 +1774,19 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" s="59" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="60"/>
       <c r="D8" s="61"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
@@ -1803,105 +1803,105 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
         <v>20</v>
       </c>
@@ -1929,13 +1929,28 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100967ABC5D75E84B4D83B4DA6CE14CDD56" ma:contentTypeVersion="2" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="037fd1e7f02219cdf2c9a7896115b454">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cd2c0e84-510c-4eda-b9bd-65693ac9c520" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a6b80e4828ccc48fd3b1dcd636bea45" ns2:_="">
     <xsd:import namespace="cd2c0e84-510c-4eda-b9bd-65693ac9c520"/>
@@ -2067,22 +2082,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8F4AE54-98C7-4760-AAC0-4CA6EA3F0EAF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68D5C62D-9B70-473D-8006-F751DF999877}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11C9FF17-37F2-40EC-91E9-E552ED4442A1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2098,21 +2115,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68D5C62D-9B70-473D-8006-F751DF999877}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8F4AE54-98C7-4760-AAC0-4CA6EA3F0EAF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>